<commit_message>
Uren Registratie en Asset List update
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -1231,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,15 +1300,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.65277777777777779</v>
+        <v>0.66216216216216217</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
@@ -1344,11 +1344,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.98611111111111116</v>
+        <v>0.98648648648648651</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1384,11 +1384,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
-        <v>0.94444444444444442</v>
+        <v>0.94594594594594594</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>44</v>
@@ -1424,11 +1424,11 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.88194444444444442</v>
+        <v>0.8783783783783784</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
@@ -1466,11 +1466,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="65">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>0.90277777777777779</v>
+        <v>0.90540540540540537</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
@@ -1508,11 +1508,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="66">
         <f>H8+H87+H24+H32+H47+H55+H63+H71+H79+H95+H103+H118+H126+H134+H142+H150+H158+H166+H174+H16</f>
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.71527777777777779</v>
+        <v>0.71621621621621623</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.57638888888888884</v>
+        <v>0.56081081081081086</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.6597222222222214</v>
+        <v>5.6554054054054053</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3404,22 +3404,22 @@
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D82" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E82" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F82" s="48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G82" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H82" s="48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I82" s="49">
         <v>0</v>
@@ -3548,31 +3548,31 @@
         <v>5</v>
       </c>
       <c r="B87" s="45">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C87" s="90">
         <f t="shared" ref="C87:G87" si="9">SUM(C82:C86)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D87" s="91">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E87" s="91">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F87" s="91">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G87" s="91">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H87" s="91">
         <f>SUM(H82:H86)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I87" s="92">
         <f>SUM(I82:I86)</f>

</xml_diff>

<commit_message>
Uren Registratie en prezi
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -1231,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K92" sqref="K92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,15 +1300,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.68604651162790697</v>
+        <v>0.67777777777777781</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
@@ -1344,11 +1344,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.98837209302325579</v>
+        <v>0.98333333333333328</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
@@ -1384,11 +1384,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
-        <v>0.93023255813953487</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>44</v>
@@ -1424,11 +1424,11 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.88953488372093026</v>
+        <v>0.89444444444444449</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>0.89534883720930236</v>
+        <v>0.85555555555555551</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
@@ -1508,11 +1508,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="66">
         <f>H8+H87+H24+H32+H47+H55+H63+H71+H79+H95+H103+H118+H126+H134+H142+H150+H158+H166+H174+H16</f>
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.73837209302325579</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.56976744186046513</v>
+        <v>0.5444444444444444</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.6976744186046506</v>
+        <v>5.6111111111111107</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3730,13 +3730,13 @@
         <v>0</v>
       </c>
       <c r="D94" s="106">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E94" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F94" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G94" s="106">
         <v>0</v>
@@ -3755,7 +3755,7 @@
         <v>5</v>
       </c>
       <c r="B95" s="45">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C95" s="90">
         <f t="shared" ref="C95:G95" si="10">SUM(C90:C94)</f>
@@ -3763,15 +3763,15 @@
       </c>
       <c r="D95" s="91">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E95" s="91">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F95" s="91">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G95" s="91">
         <f t="shared" si="10"/>
@@ -3818,22 +3818,22 @@
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D98" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E98" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F98" s="48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G98" s="48">
         <v>0</v>
       </c>
       <c r="H98" s="48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I98" s="49">
         <v>0</v>
@@ -3962,23 +3962,23 @@
         <v>5</v>
       </c>
       <c r="B103" s="45">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C103" s="90">
         <f t="shared" ref="C103:I103" si="11">SUM(C98:C102)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D103" s="91">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E103" s="91">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F103" s="91">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G103" s="91">
         <f t="shared" si="11"/>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="H103" s="91">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I103" s="91">
         <f t="shared" si="11"/>

</xml_diff>

<commit_message>
Scrum  + aanwezigheid Stuff + Michiel aanwezigheid buff werk vakantie
Dit dus
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rief\Desktop\Github\Team-Asylum3\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\Team-Asylum3\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="59">
   <si>
     <t>Maandag</t>
   </si>
@@ -199,6 +199,9 @@
   <si>
     <t>Rief ziek</t>
   </si>
+  <si>
+    <t>Koningsdag</t>
+  </si>
 </sst>
 </file>
 
@@ -261,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +354,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,7 +575,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -945,13 +954,28 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="4" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Goed" xfId="1" builtinId="26"/>
+    <cellStyle name="Invoer" xfId="4" builtinId="20"/>
+    <cellStyle name="Neutraal" xfId="3" builtinId="28"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -967,9 +991,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1007,7 +1031,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1042,6 +1066,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1077,9 +1118,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1231,23 +1289,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K92" sqref="K92"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K123" sqref="K123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
-    <col min="3" max="9" width="10.88671875" style="114" customWidth="1"/>
-    <col min="10" max="10" width="37.6640625" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" style="114" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="33" t="s">
         <v>6</v>
       </c>
@@ -1285,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1300,21 +1358,21 @@
       <c r="J2" s="1"/>
       <c r="K2" s="45">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="L2" s="61">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="M2" s="67">
         <f>L2/K2</f>
-        <v>0.67777777777777781</v>
+        <v>0.65238095238095239</v>
       </c>
       <c r="N2" s="56" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1344,17 +1402,17 @@
       <c r="K3" s="10"/>
       <c r="L3" s="62">
         <f>D8+D16+D24+D32+D47+D55+D63+D71+D79+D87+D95+D103+D118+D126+D134+D142+D150+D158+D166+D174</f>
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="M3" s="68">
         <f>L3/K2</f>
-        <v>0.98333333333333328</v>
+        <v>0.97619047619047616</v>
       </c>
       <c r="N3" s="57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1384,7 +1442,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="M4" s="69">
         <f>L4/K2</f>
@@ -1394,7 +1452,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1424,17 +1482,17 @@
       <c r="K5" s="10"/>
       <c r="L5" s="64">
         <f>F8+F16+F24+F32+F47+F55+F63+F71+F79+F87+F95+F103+F118+F126+F134+F142+F150+F158+F166+F174</f>
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="M5" s="70">
         <f>L5/K2</f>
-        <v>0.89444444444444449</v>
+        <v>0.89523809523809528</v>
       </c>
       <c r="N5" s="59" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1466,17 +1524,17 @@
       <c r="K6" s="10"/>
       <c r="L6" s="65">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="M6" s="71">
         <f>L6/K2</f>
-        <v>0.85555555555555551</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="N6" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1508,17 +1566,17 @@
       <c r="K7" s="10"/>
       <c r="L7" s="66">
         <f>H8+H87+H24+H32+H47+H55+H63+H71+H79+H95+H103+H118+H126+H134+H142+H150+H158+H166+H174+H16</f>
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="M7" s="72">
         <f>L7/K2</f>
-        <v>0.72222222222222221</v>
+        <v>0.74761904761904763</v>
       </c>
       <c r="N7" s="60" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1557,17 +1615,17 @@
       <c r="K8" s="10"/>
       <c r="L8" s="51">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="M8" s="52">
         <f>L8/K2</f>
-        <v>0.5444444444444444</v>
+        <v>0.74285714285714288</v>
       </c>
       <c r="N8" s="55" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
       <c r="E9" s="93"/>
@@ -1577,7 +1635,7 @@
       <c r="I9" s="93"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="73" t="s">
         <v>12</v>
       </c>
@@ -1596,10 +1654,10 @@
       </c>
       <c r="M10" s="40">
         <f>SUM(M2:M9)</f>
-        <v>5.6111111111111107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>5.8142857142857141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="74" t="s">
         <v>0</v>
       </c>
@@ -1623,14 +1681,14 @@
         <v>3</v>
       </c>
       <c r="I11" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J11" s="77" t="s">
         <v>50</v>
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>1</v>
       </c>
@@ -1665,7 +1723,7 @@
       </c>
       <c r="M12" s="119"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
         <v>2</v>
       </c>
@@ -1700,7 +1758,7 @@
       </c>
       <c r="M13" s="125"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
         <v>3</v>
       </c>
@@ -1735,7 +1793,7 @@
       </c>
       <c r="M14" s="126"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="75" t="s">
         <v>4</v>
       </c>
@@ -1770,7 +1828,7 @@
       </c>
       <c r="M15" s="127"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="75" t="s">
         <v>5</v>
       </c>
@@ -1803,7 +1861,7 @@
       </c>
       <c r="I16" s="91">
         <f>SUM(I11:I15)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J16" s="78"/>
       <c r="K16" s="10"/>
@@ -1812,7 +1870,7 @@
       </c>
       <c r="M16" s="128"/>
     </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="93"/>
       <c r="D17" s="93"/>
       <c r="E17" s="93"/>
@@ -1823,7 +1881,7 @@
       <c r="J17" s="13"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1838,7 +1896,7 @@
       <c r="J18" s="76"/>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -1862,14 +1920,14 @@
         <v>0</v>
       </c>
       <c r="I19" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J19" s="77" t="s">
         <v>54</v>
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
@@ -1900,7 +1958,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -1931,7 +1989,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -1962,7 +2020,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -1991,7 +2049,7 @@
       <c r="J23" s="77"/>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -2024,12 +2082,12 @@
       </c>
       <c r="I24" s="91">
         <f>SUM(I19:I23)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J24" s="38"/>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
       <c r="E25" s="93"/>
@@ -2038,7 +2096,7 @@
       <c r="H25" s="93"/>
       <c r="I25" s="93"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -2053,7 +2111,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -2077,12 +2135,12 @@
         <v>4</v>
       </c>
       <c r="I27" s="138">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
@@ -2111,7 +2169,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -2134,13 +2192,13 @@
       <c r="H29" s="132">
         <v>6</v>
       </c>
-      <c r="I29" s="133">
+      <c r="I29" s="119">
         <v>6</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2169,7 +2227,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
@@ -2198,7 +2256,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
@@ -2231,12 +2289,12 @@
       </c>
       <c r="I32" s="91">
         <f>SUM(I27:I31)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J32" s="38"/>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="93"/>
       <c r="D33" s="93"/>
       <c r="E33" s="93"/>
@@ -2245,7 +2303,7 @@
       <c r="H33" s="93"/>
       <c r="I33" s="93"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>15</v>
       </c>
@@ -2260,7 +2318,7 @@
       <c r="J34" s="16"/>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>0</v>
       </c>
@@ -2275,7 +2333,7 @@
       <c r="J35" s="18"/>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>1</v>
       </c>
@@ -2290,7 +2348,7 @@
       <c r="J36" s="18"/>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>2</v>
       </c>
@@ -2307,7 +2365,7 @@
       <c r="J37" s="18"/>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>3</v>
       </c>
@@ -2322,7 +2380,7 @@
       <c r="J38" s="18"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="32" t="s">
         <v>4</v>
       </c>
@@ -2337,7 +2395,7 @@
       <c r="J39" s="20"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="93"/>
       <c r="D40" s="93"/>
       <c r="E40" s="93"/>
@@ -2346,7 +2404,7 @@
       <c r="H40" s="93"/>
       <c r="I40" s="93"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
@@ -2361,7 +2419,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
@@ -2390,7 +2448,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>1</v>
       </c>
@@ -2419,7 +2477,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
@@ -2448,7 +2506,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>3</v>
       </c>
@@ -2477,7 +2535,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>4</v>
       </c>
@@ -2506,7 +2564,7 @@
       <c r="J46" s="3"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>5</v>
       </c>
@@ -2544,7 +2602,7 @@
       <c r="J47" s="38"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="93"/>
       <c r="D48" s="93"/>
       <c r="E48" s="93"/>
@@ -2553,7 +2611,7 @@
       <c r="H48" s="93"/>
       <c r="I48" s="93"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>17</v>
       </c>
@@ -2568,7 +2626,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>0</v>
       </c>
@@ -2597,7 +2655,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>1</v>
       </c>
@@ -2620,13 +2678,13 @@
       <c r="H51" s="132">
         <v>3</v>
       </c>
-      <c r="I51" s="49">
-        <v>0</v>
+      <c r="I51" s="133">
+        <v>3</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>2</v>
       </c>
@@ -2649,13 +2707,13 @@
       <c r="H52" s="132">
         <v>2</v>
       </c>
-      <c r="I52" s="49">
-        <v>0</v>
+      <c r="I52" s="133">
+        <v>2</v>
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>3</v>
       </c>
@@ -2684,7 +2742,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="10"/>
     </row>
-    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>4</v>
       </c>
@@ -2713,7 +2771,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="10"/>
     </row>
-    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>5</v>
       </c>
@@ -2746,12 +2804,12 @@
       </c>
       <c r="I55" s="92">
         <f>SUM(I50:I54)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J55" s="43"/>
       <c r="K55" s="10"/>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="93"/>
       <c r="D56" s="93"/>
       <c r="E56" s="93"/>
@@ -2760,7 +2818,7 @@
       <c r="H56" s="93"/>
       <c r="I56" s="93"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>18</v>
       </c>
@@ -2775,7 +2833,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="10"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>0</v>
       </c>
@@ -2804,7 +2862,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="10"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
@@ -2828,12 +2886,12 @@
         <v>0</v>
       </c>
       <c r="I59" s="145">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="10"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>2</v>
       </c>
@@ -2841,28 +2899,28 @@
       <c r="C60" s="47">
         <v>0</v>
       </c>
-      <c r="D60" s="48">
-        <v>2</v>
-      </c>
-      <c r="E60" s="48">
-        <v>2</v>
-      </c>
-      <c r="F60" s="48">
-        <v>2</v>
-      </c>
-      <c r="G60" s="48">
-        <v>2</v>
-      </c>
-      <c r="H60" s="48">
-        <v>0</v>
-      </c>
-      <c r="I60" s="49">
-        <v>0</v>
+      <c r="D60" s="132">
+        <v>2</v>
+      </c>
+      <c r="E60" s="132">
+        <v>2</v>
+      </c>
+      <c r="F60" s="132">
+        <v>2</v>
+      </c>
+      <c r="G60" s="132">
+        <v>2</v>
+      </c>
+      <c r="H60" s="132">
+        <v>0</v>
+      </c>
+      <c r="I60" s="133">
+        <v>2</v>
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="10"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>3</v>
       </c>
@@ -2870,13 +2928,13 @@
       <c r="C61" s="47">
         <v>0</v>
       </c>
-      <c r="D61" s="48">
-        <v>2</v>
-      </c>
-      <c r="E61" s="48">
-        <v>2</v>
-      </c>
-      <c r="F61" s="48">
+      <c r="D61" s="132">
+        <v>2</v>
+      </c>
+      <c r="E61" s="132">
+        <v>2</v>
+      </c>
+      <c r="F61" s="132">
         <v>2</v>
       </c>
       <c r="G61" s="48">
@@ -2885,13 +2943,13 @@
       <c r="H61" s="48">
         <v>0</v>
       </c>
-      <c r="I61" s="49">
-        <v>0</v>
+      <c r="I61" s="133">
+        <v>2</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="10"/>
     </row>
-    <row r="62" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>4</v>
       </c>
@@ -2920,7 +2978,7 @@
       <c r="J62" s="3"/>
       <c r="K62" s="10"/>
     </row>
-    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>5</v>
       </c>
@@ -2953,12 +3011,12 @@
       </c>
       <c r="I63" s="92">
         <f>SUM(I58:I62)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J63" s="43"/>
       <c r="K63" s="10"/>
     </row>
-    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="10"/>
       <c r="C64" s="109"/>
       <c r="D64" s="109"/>
@@ -2969,7 +3027,7 @@
       <c r="I64" s="109"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>19</v>
       </c>
@@ -2984,7 +3042,7 @@
       <c r="J65" s="23"/>
       <c r="K65" s="10"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>0</v>
       </c>
@@ -3013,7 +3071,7 @@
       <c r="J66" s="25"/>
       <c r="K66" s="10"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>1</v>
       </c>
@@ -3042,7 +3100,7 @@
       <c r="J67" s="25"/>
       <c r="K67" s="10"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>2</v>
       </c>
@@ -3071,70 +3129,70 @@
       <c r="J68" s="25"/>
       <c r="K68" s="10"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B69" s="35"/>
-      <c r="C69" s="47">
-        <v>2</v>
-      </c>
-      <c r="D69" s="48">
-        <v>2</v>
-      </c>
-      <c r="E69" s="48">
-        <v>2</v>
-      </c>
-      <c r="F69" s="48">
-        <v>2</v>
-      </c>
-      <c r="G69" s="48">
-        <v>2</v>
-      </c>
-      <c r="H69" s="48">
-        <v>2</v>
-      </c>
-      <c r="I69" s="49">
+      <c r="C69" s="131">
+        <v>2</v>
+      </c>
+      <c r="D69" s="132">
+        <v>2</v>
+      </c>
+      <c r="E69" s="132">
+        <v>2</v>
+      </c>
+      <c r="F69" s="132">
+        <v>2</v>
+      </c>
+      <c r="G69" s="132">
+        <v>2</v>
+      </c>
+      <c r="H69" s="132">
+        <v>2</v>
+      </c>
+      <c r="I69" s="133">
         <v>1</v>
       </c>
       <c r="J69" s="25"/>
       <c r="K69" s="10"/>
     </row>
-    <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B70" s="36"/>
-      <c r="C70" s="108">
-        <v>4</v>
-      </c>
-      <c r="D70" s="106">
-        <v>4</v>
-      </c>
-      <c r="E70" s="106">
-        <v>4</v>
-      </c>
-      <c r="F70" s="106">
-        <v>4</v>
-      </c>
-      <c r="G70" s="106">
-        <v>4</v>
-      </c>
-      <c r="H70" s="106">
+      <c r="C70" s="137">
+        <v>4</v>
+      </c>
+      <c r="D70" s="135">
+        <v>4</v>
+      </c>
+      <c r="E70" s="135">
+        <v>4</v>
+      </c>
+      <c r="F70" s="135">
+        <v>4</v>
+      </c>
+      <c r="G70" s="135">
+        <v>4</v>
+      </c>
+      <c r="H70" s="135">
         <v>3</v>
       </c>
-      <c r="I70" s="107">
-        <v>0</v>
+      <c r="I70" s="136">
+        <v>3</v>
       </c>
       <c r="J70" s="27"/>
       <c r="K70" s="10"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B71" s="45">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C71" s="90">
         <f t="shared" ref="C71:G71" si="7">SUM(C66:C70)</f>
@@ -3162,12 +3220,12 @@
       </c>
       <c r="I71" s="92">
         <f>SUM(I66:I70)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J71" s="43"/>
       <c r="K71" s="10"/>
     </row>
-    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C72" s="93"/>
       <c r="D72" s="93"/>
       <c r="E72" s="93"/>
@@ -3176,7 +3234,7 @@
       <c r="H72" s="93"/>
       <c r="I72" s="93"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>20</v>
       </c>
@@ -3191,27 +3249,27 @@
       <c r="J73" s="1"/>
       <c r="K73" s="10"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B74" s="10"/>
-      <c r="C74" s="47">
-        <v>4</v>
-      </c>
-      <c r="D74" s="48">
-        <v>4</v>
-      </c>
-      <c r="E74" s="48">
-        <v>4</v>
-      </c>
-      <c r="F74" s="48">
-        <v>4</v>
-      </c>
-      <c r="G74" s="48">
-        <v>4</v>
-      </c>
-      <c r="H74" s="48">
+      <c r="C74" s="131">
+        <v>4</v>
+      </c>
+      <c r="D74" s="132">
+        <v>4</v>
+      </c>
+      <c r="E74" s="132">
+        <v>4</v>
+      </c>
+      <c r="F74" s="132">
+        <v>4</v>
+      </c>
+      <c r="G74" s="132">
+        <v>4</v>
+      </c>
+      <c r="H74" s="132">
         <v>4</v>
       </c>
       <c r="I74" s="49">
@@ -3220,36 +3278,36 @@
       <c r="J74" s="2"/>
       <c r="K74" s="10"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B75" s="10"/>
-      <c r="C75" s="47">
-        <v>4</v>
-      </c>
-      <c r="D75" s="48">
+      <c r="C75" s="131">
+        <v>4</v>
+      </c>
+      <c r="D75" s="132">
         <v>4</v>
       </c>
       <c r="E75" s="48">
         <v>0</v>
       </c>
-      <c r="F75" s="48">
-        <v>4</v>
-      </c>
-      <c r="G75" s="48">
-        <v>4</v>
-      </c>
-      <c r="H75" s="48">
-        <v>4</v>
-      </c>
-      <c r="I75" s="49">
-        <v>4</v>
+      <c r="F75" s="132">
+        <v>4</v>
+      </c>
+      <c r="G75" s="132">
+        <v>4</v>
+      </c>
+      <c r="H75" s="132">
+        <v>4</v>
+      </c>
+      <c r="I75" s="133">
+        <v>3</v>
       </c>
       <c r="J75" s="2"/>
       <c r="K75" s="10"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>2</v>
       </c>
@@ -3257,10 +3315,10 @@
       <c r="C76" s="47">
         <v>0</v>
       </c>
-      <c r="D76" s="48">
-        <v>2</v>
-      </c>
-      <c r="E76" s="48">
+      <c r="D76" s="132">
+        <v>2</v>
+      </c>
+      <c r="E76" s="132">
         <v>2</v>
       </c>
       <c r="F76" s="48">
@@ -3269,7 +3327,7 @@
       <c r="G76" s="48">
         <v>0</v>
       </c>
-      <c r="H76" s="48">
+      <c r="H76" s="132">
         <v>2</v>
       </c>
       <c r="I76" s="49">
@@ -3278,27 +3336,27 @@
       <c r="J76" s="2"/>
       <c r="K76" s="10"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B77" s="10"/>
-      <c r="C77" s="47">
-        <v>2</v>
-      </c>
-      <c r="D77" s="48">
-        <v>2</v>
-      </c>
-      <c r="E77" s="48">
+      <c r="C77" s="131">
+        <v>2</v>
+      </c>
+      <c r="D77" s="132">
+        <v>2</v>
+      </c>
+      <c r="E77" s="132">
         <v>2</v>
       </c>
       <c r="F77" s="48">
         <v>0</v>
       </c>
-      <c r="G77" s="48">
-        <v>2</v>
-      </c>
-      <c r="H77" s="48">
+      <c r="G77" s="132">
+        <v>2</v>
+      </c>
+      <c r="H77" s="132">
         <v>1</v>
       </c>
       <c r="I77" s="49">
@@ -3307,27 +3365,27 @@
       <c r="J77" s="2"/>
       <c r="K77" s="10"/>
     </row>
-    <row r="78" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B78" s="9"/>
-      <c r="C78" s="108">
-        <v>4</v>
-      </c>
-      <c r="D78" s="106">
-        <v>4</v>
-      </c>
-      <c r="E78" s="106">
+      <c r="C78" s="137">
+        <v>4</v>
+      </c>
+      <c r="D78" s="135">
+        <v>4</v>
+      </c>
+      <c r="E78" s="135">
         <v>4</v>
       </c>
       <c r="F78" s="106">
         <v>0</v>
       </c>
-      <c r="G78" s="106">
-        <v>4</v>
-      </c>
-      <c r="H78" s="106">
+      <c r="G78" s="135">
+        <v>4</v>
+      </c>
+      <c r="H78" s="135">
         <v>3</v>
       </c>
       <c r="I78" s="107">
@@ -3336,7 +3394,7 @@
       <c r="J78" s="3"/>
       <c r="K78" s="10"/>
     </row>
-    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>5</v>
       </c>
@@ -3369,12 +3427,12 @@
       </c>
       <c r="I79" s="92">
         <f>SUM(I74:I78)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J79" s="43"/>
       <c r="K79" s="10"/>
     </row>
-    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="93"/>
       <c r="D80" s="93"/>
       <c r="E80" s="93"/>
@@ -3383,7 +3441,7 @@
       <c r="H80" s="93"/>
       <c r="I80" s="93"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>21</v>
       </c>
@@ -3398,27 +3456,27 @@
       <c r="J81" s="1"/>
       <c r="K81" s="10"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B82" s="10"/>
-      <c r="C82" s="47">
-        <v>4</v>
-      </c>
-      <c r="D82" s="48">
-        <v>4</v>
-      </c>
-      <c r="E82" s="48">
-        <v>4</v>
-      </c>
-      <c r="F82" s="48">
+      <c r="C82" s="131">
+        <v>4</v>
+      </c>
+      <c r="D82" s="132">
+        <v>4</v>
+      </c>
+      <c r="E82" s="132">
+        <v>4</v>
+      </c>
+      <c r="F82" s="132">
         <v>3</v>
       </c>
-      <c r="G82" s="48">
-        <v>4</v>
-      </c>
-      <c r="H82" s="48">
+      <c r="G82" s="132">
+        <v>4</v>
+      </c>
+      <c r="H82" s="132">
         <v>3</v>
       </c>
       <c r="I82" s="49">
@@ -3427,114 +3485,114 @@
       <c r="J82" s="2"/>
       <c r="K82" s="10"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B83" s="10"/>
-      <c r="C83" s="47">
-        <v>4</v>
-      </c>
-      <c r="D83" s="48">
+      <c r="C83" s="131">
+        <v>4</v>
+      </c>
+      <c r="D83" s="132">
         <v>4</v>
       </c>
       <c r="E83" s="48">
         <v>0</v>
       </c>
-      <c r="F83" s="48">
-        <v>4</v>
-      </c>
-      <c r="G83" s="48">
-        <v>2</v>
-      </c>
-      <c r="H83" s="48">
-        <v>4</v>
-      </c>
-      <c r="I83" s="49">
+      <c r="F83" s="132">
+        <v>4</v>
+      </c>
+      <c r="G83" s="132">
+        <v>2</v>
+      </c>
+      <c r="H83" s="132">
+        <v>4</v>
+      </c>
+      <c r="I83" s="133">
         <v>3</v>
       </c>
       <c r="J83" s="2"/>
       <c r="K83" s="10"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B84" s="10"/>
-      <c r="C84" s="47">
-        <v>2</v>
-      </c>
-      <c r="D84" s="48">
-        <v>2</v>
-      </c>
-      <c r="E84" s="48">
-        <v>2</v>
-      </c>
-      <c r="F84" s="48">
-        <v>2</v>
-      </c>
-      <c r="G84" s="48">
-        <v>2</v>
-      </c>
-      <c r="H84" s="48">
-        <v>2</v>
-      </c>
-      <c r="I84" s="49">
+      <c r="C84" s="131">
+        <v>2</v>
+      </c>
+      <c r="D84" s="132">
+        <v>2</v>
+      </c>
+      <c r="E84" s="132">
+        <v>2</v>
+      </c>
+      <c r="F84" s="132">
+        <v>2</v>
+      </c>
+      <c r="G84" s="132">
+        <v>2</v>
+      </c>
+      <c r="H84" s="132">
+        <v>2</v>
+      </c>
+      <c r="I84" s="133">
         <v>2</v>
       </c>
       <c r="J84" s="2"/>
       <c r="K84" s="10"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B85" s="10"/>
-      <c r="C85" s="47">
-        <v>2</v>
-      </c>
-      <c r="D85" s="48">
-        <v>2</v>
-      </c>
-      <c r="E85" s="48">
-        <v>2</v>
-      </c>
-      <c r="F85" s="48">
+      <c r="C85" s="131">
+        <v>2</v>
+      </c>
+      <c r="D85" s="132">
+        <v>2</v>
+      </c>
+      <c r="E85" s="132">
+        <v>2</v>
+      </c>
+      <c r="F85" s="132">
         <v>2</v>
       </c>
       <c r="G85" s="48">
         <v>0</v>
       </c>
-      <c r="H85" s="48">
-        <v>2</v>
-      </c>
-      <c r="I85" s="49">
+      <c r="H85" s="132">
+        <v>2</v>
+      </c>
+      <c r="I85" s="133">
         <v>2</v>
       </c>
       <c r="J85" s="2"/>
       <c r="K85" s="10"/>
     </row>
-    <row r="86" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B86" s="9"/>
-      <c r="C86" s="108">
-        <v>4</v>
-      </c>
-      <c r="D86" s="106">
-        <v>4</v>
-      </c>
-      <c r="E86" s="106">
-        <v>4</v>
-      </c>
-      <c r="F86" s="106">
+      <c r="C86" s="137">
+        <v>4</v>
+      </c>
+      <c r="D86" s="135">
+        <v>4</v>
+      </c>
+      <c r="E86" s="135">
+        <v>4</v>
+      </c>
+      <c r="F86" s="135">
         <v>3</v>
       </c>
-      <c r="G86" s="106">
-        <v>4</v>
-      </c>
-      <c r="H86" s="106">
+      <c r="G86" s="135">
+        <v>4</v>
+      </c>
+      <c r="H86" s="135">
         <v>3</v>
       </c>
       <c r="I86" s="107">
@@ -3543,7 +3601,7 @@
       <c r="J86" s="3"/>
       <c r="K86" s="10"/>
     </row>
-    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>5</v>
       </c>
@@ -3581,7 +3639,7 @@
       <c r="J87" s="43"/>
       <c r="K87" s="10"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="93"/>
       <c r="D88" s="93"/>
       <c r="E88" s="93"/>
@@ -3590,7 +3648,7 @@
       <c r="H88" s="93"/>
       <c r="I88" s="93"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>22</v>
       </c>
@@ -3605,7 +3663,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="10"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>0</v>
       </c>
@@ -3613,115 +3671,115 @@
       <c r="C90" s="47">
         <v>0</v>
       </c>
-      <c r="D90" s="48">
-        <v>4</v>
-      </c>
-      <c r="E90" s="48">
-        <v>4</v>
-      </c>
-      <c r="F90" s="48">
-        <v>4</v>
-      </c>
-      <c r="G90" s="48">
-        <v>4</v>
-      </c>
-      <c r="H90" s="48">
-        <v>4</v>
-      </c>
-      <c r="I90" s="49">
-        <v>0</v>
+      <c r="D90" s="132">
+        <v>4</v>
+      </c>
+      <c r="E90" s="132">
+        <v>4</v>
+      </c>
+      <c r="F90" s="132">
+        <v>4</v>
+      </c>
+      <c r="G90" s="132">
+        <v>4</v>
+      </c>
+      <c r="H90" s="132">
+        <v>4</v>
+      </c>
+      <c r="I90" s="133">
+        <v>4</v>
       </c>
       <c r="J90" s="2"/>
       <c r="K90" s="10"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B91" s="10"/>
-      <c r="C91" s="47">
-        <v>4</v>
-      </c>
-      <c r="D91" s="48">
-        <v>4</v>
-      </c>
-      <c r="E91" s="48">
-        <v>4</v>
-      </c>
-      <c r="F91" s="48">
-        <v>4</v>
-      </c>
-      <c r="G91" s="48">
-        <v>4</v>
-      </c>
-      <c r="H91" s="48">
-        <v>4</v>
-      </c>
-      <c r="I91" s="49">
+      <c r="C91" s="131">
+        <v>4</v>
+      </c>
+      <c r="D91" s="132">
+        <v>4</v>
+      </c>
+      <c r="E91" s="132">
+        <v>4</v>
+      </c>
+      <c r="F91" s="132">
+        <v>4</v>
+      </c>
+      <c r="G91" s="132">
+        <v>4</v>
+      </c>
+      <c r="H91" s="132">
+        <v>4</v>
+      </c>
+      <c r="I91" s="133">
         <v>4</v>
       </c>
       <c r="J91" s="2"/>
       <c r="K91" s="10"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B92" s="10"/>
-      <c r="C92" s="47">
-        <v>2</v>
-      </c>
-      <c r="D92" s="48">
-        <v>2</v>
-      </c>
-      <c r="E92" s="48">
-        <v>2</v>
-      </c>
-      <c r="F92" s="48">
-        <v>2</v>
-      </c>
-      <c r="G92" s="48">
+      <c r="C92" s="131">
+        <v>2</v>
+      </c>
+      <c r="D92" s="132">
+        <v>2</v>
+      </c>
+      <c r="E92" s="132">
+        <v>2</v>
+      </c>
+      <c r="F92" s="132">
+        <v>2</v>
+      </c>
+      <c r="G92" s="132">
         <v>2</v>
       </c>
       <c r="H92" s="48">
         <v>0</v>
       </c>
-      <c r="I92" s="49">
+      <c r="I92" s="133">
         <v>2</v>
       </c>
       <c r="J92" s="2"/>
       <c r="K92" s="10"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B93" s="10"/>
-      <c r="C93" s="47">
-        <v>2</v>
-      </c>
-      <c r="D93" s="48">
-        <v>2</v>
-      </c>
-      <c r="E93" s="48">
-        <v>2</v>
-      </c>
-      <c r="F93" s="48">
-        <v>2</v>
-      </c>
-      <c r="G93" s="48">
-        <v>2</v>
-      </c>
-      <c r="H93" s="48">
-        <v>2</v>
-      </c>
-      <c r="I93" s="49">
+      <c r="C93" s="131">
+        <v>2</v>
+      </c>
+      <c r="D93" s="132">
+        <v>2</v>
+      </c>
+      <c r="E93" s="132">
+        <v>2</v>
+      </c>
+      <c r="F93" s="132">
+        <v>2</v>
+      </c>
+      <c r="G93" s="132">
+        <v>2</v>
+      </c>
+      <c r="H93" s="132">
+        <v>2</v>
+      </c>
+      <c r="I93" s="133">
         <v>2</v>
       </c>
       <c r="J93" s="2"/>
       <c r="K93" s="10"/>
     </row>
-    <row r="94" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>4</v>
       </c>
@@ -3729,13 +3787,13 @@
       <c r="C94" s="108">
         <v>0</v>
       </c>
-      <c r="D94" s="106">
+      <c r="D94" s="135">
         <v>3</v>
       </c>
-      <c r="E94" s="106">
-        <v>4</v>
-      </c>
-      <c r="F94" s="106">
+      <c r="E94" s="135">
+        <v>4</v>
+      </c>
+      <c r="F94" s="135">
         <v>4</v>
       </c>
       <c r="G94" s="106">
@@ -3744,13 +3802,13 @@
       <c r="H94" s="106">
         <v>0</v>
       </c>
-      <c r="I94" s="107">
-        <v>0</v>
+      <c r="I94" s="136">
+        <v>4</v>
       </c>
       <c r="J94" s="3"/>
       <c r="K94" s="10"/>
     </row>
-    <row r="95" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>5</v>
       </c>
@@ -3783,12 +3841,12 @@
       </c>
       <c r="I95" s="92">
         <f>SUM(I90:I94)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J95" s="43"/>
       <c r="K95" s="10"/>
     </row>
-    <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C96" s="93"/>
       <c r="D96" s="93"/>
       <c r="E96" s="93"/>
@@ -3797,7 +3855,7 @@
       <c r="H96" s="93"/>
       <c r="I96" s="93"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>23</v>
       </c>
@@ -3812,190 +3870,192 @@
       <c r="J97" s="1"/>
       <c r="K97" s="10"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B98" s="10"/>
-      <c r="C98" s="47">
-        <v>4</v>
-      </c>
-      <c r="D98" s="48">
-        <v>4</v>
-      </c>
-      <c r="E98" s="48">
-        <v>4</v>
-      </c>
-      <c r="F98" s="48">
+      <c r="C98" s="131">
+        <v>4</v>
+      </c>
+      <c r="D98" s="132">
+        <v>4</v>
+      </c>
+      <c r="E98" s="132">
+        <v>4</v>
+      </c>
+      <c r="F98" s="132">
         <v>4</v>
       </c>
       <c r="G98" s="48">
         <v>0</v>
       </c>
-      <c r="H98" s="48">
+      <c r="H98" s="132">
         <v>3</v>
       </c>
-      <c r="I98" s="49">
-        <v>0</v>
+      <c r="I98" s="133">
+        <v>4</v>
       </c>
       <c r="J98" s="2"/>
       <c r="K98" s="10"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B99" s="10"/>
-      <c r="C99" s="47">
-        <v>0</v>
-      </c>
-      <c r="D99" s="48">
-        <v>0</v>
-      </c>
-      <c r="E99" s="48">
-        <v>0</v>
-      </c>
-      <c r="F99" s="48">
-        <v>0</v>
-      </c>
-      <c r="G99" s="48">
-        <v>0</v>
-      </c>
-      <c r="H99" s="48">
-        <v>0</v>
-      </c>
-      <c r="I99" s="49">
-        <v>0</v>
+      <c r="C99" s="131">
+        <v>3</v>
+      </c>
+      <c r="D99" s="132">
+        <v>4</v>
+      </c>
+      <c r="E99" s="132">
+        <v>4</v>
+      </c>
+      <c r="F99" s="132">
+        <v>4</v>
+      </c>
+      <c r="G99" s="132">
+        <v>4</v>
+      </c>
+      <c r="H99" s="132">
+        <v>4</v>
+      </c>
+      <c r="I99" s="133">
+        <v>4</v>
       </c>
       <c r="J99" s="2"/>
       <c r="K99" s="10"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B100" s="10"/>
-      <c r="C100" s="47">
-        <v>0</v>
-      </c>
-      <c r="D100" s="48">
-        <v>0</v>
-      </c>
-      <c r="E100" s="48">
-        <v>0</v>
-      </c>
-      <c r="F100" s="48">
-        <v>0</v>
-      </c>
-      <c r="G100" s="48">
-        <v>0</v>
-      </c>
-      <c r="H100" s="48">
-        <v>0</v>
-      </c>
-      <c r="I100" s="49">
-        <v>0</v>
-      </c>
-      <c r="J100" s="2"/>
+      <c r="C100" s="131">
+        <v>4</v>
+      </c>
+      <c r="D100" s="132">
+        <v>4</v>
+      </c>
+      <c r="E100" s="132">
+        <v>4</v>
+      </c>
+      <c r="F100" s="132">
+        <v>4</v>
+      </c>
+      <c r="G100" s="132">
+        <v>4</v>
+      </c>
+      <c r="H100" s="132">
+        <v>4</v>
+      </c>
+      <c r="I100" s="133">
+        <v>4</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="K100" s="10"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B101" s="10"/>
-      <c r="C101" s="47">
-        <v>0</v>
-      </c>
-      <c r="D101" s="48">
-        <v>0</v>
-      </c>
-      <c r="E101" s="48">
-        <v>0</v>
-      </c>
-      <c r="F101" s="48">
-        <v>0</v>
-      </c>
-      <c r="G101" s="48">
-        <v>0</v>
-      </c>
-      <c r="H101" s="48">
-        <v>0</v>
-      </c>
-      <c r="I101" s="49">
-        <v>0</v>
+      <c r="C101" s="131">
+        <v>4</v>
+      </c>
+      <c r="D101" s="132">
+        <v>4</v>
+      </c>
+      <c r="E101" s="132">
+        <v>4</v>
+      </c>
+      <c r="F101" s="132">
+        <v>4</v>
+      </c>
+      <c r="G101" s="132">
+        <v>4</v>
+      </c>
+      <c r="H101" s="132">
+        <v>4</v>
+      </c>
+      <c r="I101" s="133">
+        <v>4</v>
       </c>
       <c r="J101" s="2"/>
       <c r="K101" s="10"/>
     </row>
-    <row r="102" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B102" s="9"/>
-      <c r="C102" s="108">
-        <v>0</v>
-      </c>
-      <c r="D102" s="106">
-        <v>0</v>
-      </c>
-      <c r="E102" s="106">
-        <v>0</v>
-      </c>
-      <c r="F102" s="106">
-        <v>0</v>
-      </c>
-      <c r="G102" s="106">
-        <v>0</v>
-      </c>
-      <c r="H102" s="106">
-        <v>0</v>
-      </c>
-      <c r="I102" s="107">
-        <v>0</v>
+      <c r="C102" s="137">
+        <v>4</v>
+      </c>
+      <c r="D102" s="135">
+        <v>4</v>
+      </c>
+      <c r="E102" s="135">
+        <v>4</v>
+      </c>
+      <c r="F102" s="135">
+        <v>4</v>
+      </c>
+      <c r="G102" s="135">
+        <v>4</v>
+      </c>
+      <c r="H102" s="135">
+        <v>4</v>
+      </c>
+      <c r="I102" s="136">
+        <v>4</v>
       </c>
       <c r="J102" s="3"/>
       <c r="K102" s="10"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B103" s="45">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C103" s="90">
         <f t="shared" ref="C103:I103" si="11">SUM(C98:C102)</f>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D103" s="91">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E103" s="91">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F103" s="91">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G103" s="91">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H103" s="91">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="I103" s="91">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J103" s="38"/>
       <c r="K103" s="10"/>
     </row>
-    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C104" s="93"/>
       <c r="D104" s="93"/>
       <c r="E104" s="93"/>
@@ -4004,7 +4064,7 @@
       <c r="H104" s="93"/>
       <c r="I104" s="93"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="30" t="s">
         <v>24</v>
       </c>
@@ -4019,7 +4079,7 @@
       <c r="J105" s="16"/>
       <c r="K105" s="10"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="31" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4094,7 @@
       <c r="J106" s="18"/>
       <c r="K106" s="10"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="31" t="s">
         <v>1</v>
       </c>
@@ -4049,7 +4109,7 @@
       <c r="J107" s="18"/>
       <c r="K107" s="10"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="31" t="s">
         <v>2</v>
       </c>
@@ -4066,7 +4126,7 @@
       <c r="J108" s="18"/>
       <c r="K108" s="10"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="31" t="s">
         <v>3</v>
       </c>
@@ -4081,7 +4141,7 @@
       <c r="J109" s="18"/>
       <c r="K109" s="10"/>
     </row>
-    <row r="110" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="32" t="s">
         <v>4</v>
       </c>
@@ -4096,7 +4156,7 @@
       <c r="J110" s="20"/>
       <c r="K110" s="10"/>
     </row>
-    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="93"/>
       <c r="D111" s="93"/>
       <c r="E111" s="93"/>
@@ -4105,7 +4165,7 @@
       <c r="H111" s="93"/>
       <c r="I111" s="93"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>25</v>
       </c>
@@ -4120,28 +4180,28 @@
       <c r="J112" s="1"/>
       <c r="K112" s="10"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B113" s="10"/>
-      <c r="C113" s="47">
-        <v>0</v>
-      </c>
-      <c r="D113" s="48">
-        <v>0</v>
-      </c>
-      <c r="E113" s="48">
-        <v>0</v>
-      </c>
-      <c r="F113" s="48">
-        <v>0</v>
-      </c>
-      <c r="G113" s="48">
-        <v>0</v>
-      </c>
-      <c r="H113" s="48">
-        <v>0</v>
+      <c r="C113" s="146">
+        <v>0</v>
+      </c>
+      <c r="D113" s="132">
+        <v>4</v>
+      </c>
+      <c r="E113" s="132">
+        <v>4</v>
+      </c>
+      <c r="F113" s="132">
+        <v>4</v>
+      </c>
+      <c r="G113" s="132">
+        <v>4</v>
+      </c>
+      <c r="H113" s="132">
+        <v>4</v>
       </c>
       <c r="I113" s="49">
         <v>0</v>
@@ -4149,70 +4209,70 @@
       <c r="J113" s="2"/>
       <c r="K113" s="10"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B114" s="10"/>
-      <c r="C114" s="47">
-        <v>0</v>
-      </c>
-      <c r="D114" s="48">
-        <v>0</v>
-      </c>
-      <c r="E114" s="48">
-        <v>0</v>
-      </c>
-      <c r="F114" s="48">
-        <v>0</v>
-      </c>
-      <c r="G114" s="48">
-        <v>0</v>
-      </c>
-      <c r="H114" s="48">
-        <v>0</v>
-      </c>
-      <c r="I114" s="49">
-        <v>0</v>
+      <c r="C114" s="146">
+        <v>0</v>
+      </c>
+      <c r="D114" s="132">
+        <v>4</v>
+      </c>
+      <c r="E114" s="132">
+        <v>4</v>
+      </c>
+      <c r="F114" s="132">
+        <v>4</v>
+      </c>
+      <c r="G114" s="132">
+        <v>4</v>
+      </c>
+      <c r="H114" s="132">
+        <v>4</v>
+      </c>
+      <c r="I114" s="133">
+        <v>4</v>
       </c>
       <c r="J114" s="2"/>
       <c r="K114" s="10"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B115" s="10"/>
-      <c r="C115" s="47">
-        <v>0</v>
-      </c>
-      <c r="D115" s="48">
-        <v>0</v>
-      </c>
-      <c r="E115" s="48">
-        <v>0</v>
-      </c>
-      <c r="F115" s="48">
-        <v>0</v>
-      </c>
-      <c r="G115" s="48">
-        <v>0</v>
-      </c>
-      <c r="H115" s="48">
-        <v>0</v>
-      </c>
-      <c r="I115" s="49">
-        <v>0</v>
+      <c r="C115" s="146">
+        <v>0</v>
+      </c>
+      <c r="D115" s="132">
+        <v>4</v>
+      </c>
+      <c r="E115" s="132">
+        <v>4</v>
+      </c>
+      <c r="F115" s="132">
+        <v>3</v>
+      </c>
+      <c r="G115" s="132">
+        <v>4</v>
+      </c>
+      <c r="H115" s="132">
+        <v>3</v>
+      </c>
+      <c r="I115" s="133">
+        <v>4</v>
       </c>
       <c r="J115" s="2"/>
       <c r="K115" s="10"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B116" s="10"/>
-      <c r="C116" s="47">
+      <c r="C116" s="146">
         <v>0</v>
       </c>
       <c r="D116" s="48">
@@ -4236,12 +4296,12 @@
       <c r="J116" s="2"/>
       <c r="K116" s="10"/>
     </row>
-    <row r="117" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B117" s="9"/>
-      <c r="C117" s="108">
+      <c r="C117" s="147">
         <v>0</v>
       </c>
       <c r="D117" s="106">
@@ -4265,46 +4325,46 @@
       <c r="J117" s="3"/>
       <c r="K117" s="10"/>
     </row>
-    <row r="118" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B118" s="45">
-        <v>0</v>
-      </c>
-      <c r="C118" s="90">
+        <v>12</v>
+      </c>
+      <c r="C118" s="148">
         <f>SUM(C113:C117)</f>
         <v>0</v>
       </c>
       <c r="D118" s="91">
         <f t="shared" ref="D118:I118" si="12">SUM(D113:D117)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E118" s="91">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F118" s="91">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G118" s="91">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H118" s="91">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I118" s="91">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J118" s="38"/>
       <c r="K118" s="10"/>
     </row>
-    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C119" s="93"/>
+    <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C119" s="149"/>
       <c r="D119" s="93"/>
       <c r="E119" s="93"/>
       <c r="F119" s="93"/>
@@ -4312,12 +4372,12 @@
       <c r="H119" s="93"/>
       <c r="I119" s="93"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B120" s="8"/>
-      <c r="C120" s="87"/>
+      <c r="C120" s="150"/>
       <c r="D120" s="88"/>
       <c r="E120" s="88"/>
       <c r="F120" s="88"/>
@@ -4327,12 +4387,12 @@
       <c r="J120" s="1"/>
       <c r="K120" s="10"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B121" s="10"/>
-      <c r="C121" s="47">
+      <c r="C121" s="146">
         <v>0</v>
       </c>
       <c r="D121" s="48">
@@ -4356,12 +4416,12 @@
       <c r="J121" s="2"/>
       <c r="K121" s="10"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B122" s="10"/>
-      <c r="C122" s="47">
+      <c r="C122" s="146">
         <v>0</v>
       </c>
       <c r="D122" s="48">
@@ -4385,12 +4445,12 @@
       <c r="J122" s="2"/>
       <c r="K122" s="10"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B123" s="10"/>
-      <c r="C123" s="47">
+      <c r="C123" s="146">
         <v>0</v>
       </c>
       <c r="D123" s="48">
@@ -4414,12 +4474,12 @@
       <c r="J123" s="2"/>
       <c r="K123" s="10"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B124" s="10"/>
-      <c r="C124" s="47">
+      <c r="C124" s="146">
         <v>0</v>
       </c>
       <c r="D124" s="48">
@@ -4443,12 +4503,12 @@
       <c r="J124" s="2"/>
       <c r="K124" s="10"/>
     </row>
-    <row r="125" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B125" s="9"/>
-      <c r="C125" s="108">
+      <c r="C125" s="147">
         <v>0</v>
       </c>
       <c r="D125" s="106">
@@ -4472,14 +4532,14 @@
       <c r="J125" s="3"/>
       <c r="K125" s="10"/>
     </row>
-    <row r="126" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B126" s="45">
         <v>0</v>
       </c>
-      <c r="C126" s="90">
+      <c r="C126" s="148">
         <f t="shared" ref="C126:I126" si="13">SUM(C121:C125)</f>
         <v>0</v>
       </c>
@@ -4510,8 +4570,8 @@
       <c r="J126" s="38"/>
       <c r="K126" s="10"/>
     </row>
-    <row r="127" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C127" s="93"/>
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C127" s="149"/>
       <c r="D127" s="93"/>
       <c r="E127" s="93"/>
       <c r="F127" s="93"/>
@@ -4519,12 +4579,12 @@
       <c r="H127" s="93"/>
       <c r="I127" s="93"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B128" s="8"/>
-      <c r="C128" s="87"/>
+      <c r="C128" s="150"/>
       <c r="D128" s="88"/>
       <c r="E128" s="88"/>
       <c r="F128" s="88"/>
@@ -4534,12 +4594,12 @@
       <c r="J128" s="1"/>
       <c r="K128" s="10"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B129" s="10"/>
-      <c r="C129" s="47">
+      <c r="C129" s="146">
         <v>0</v>
       </c>
       <c r="D129" s="48">
@@ -4563,12 +4623,12 @@
       <c r="J129" s="2"/>
       <c r="K129" s="10"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B130" s="10"/>
-      <c r="C130" s="47">
+      <c r="C130" s="146">
         <v>0</v>
       </c>
       <c r="D130" s="48">
@@ -4592,12 +4652,12 @@
       <c r="J130" s="2"/>
       <c r="K130" s="10"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B131" s="10"/>
-      <c r="C131" s="47">
+      <c r="C131" s="146">
         <v>0</v>
       </c>
       <c r="D131" s="48">
@@ -4621,12 +4681,12 @@
       <c r="J131" s="2"/>
       <c r="K131" s="10"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B132" s="10"/>
-      <c r="C132" s="47">
+      <c r="C132" s="146">
         <v>0</v>
       </c>
       <c r="D132" s="48">
@@ -4650,12 +4710,12 @@
       <c r="J132" s="2"/>
       <c r="K132" s="10"/>
     </row>
-    <row r="133" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B133" s="9"/>
-      <c r="C133" s="108">
+      <c r="C133" s="147">
         <v>0</v>
       </c>
       <c r="D133" s="106">
@@ -4679,14 +4739,14 @@
       <c r="J133" s="3"/>
       <c r="K133" s="10"/>
     </row>
-    <row r="134" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B134" s="45">
         <v>0</v>
       </c>
-      <c r="C134" s="90">
+      <c r="C134" s="148">
         <f t="shared" ref="C134:I134" si="14">SUM(C129:C133)</f>
         <v>0</v>
       </c>
@@ -4717,8 +4777,8 @@
       <c r="J134" s="38"/>
       <c r="K134" s="10"/>
     </row>
-    <row r="135" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C135" s="93"/>
+    <row r="135" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C135" s="149"/>
       <c r="D135" s="93"/>
       <c r="E135" s="93"/>
       <c r="F135" s="93"/>
@@ -4726,12 +4786,12 @@
       <c r="H135" s="93"/>
       <c r="I135" s="93"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B136" s="22"/>
-      <c r="C136" s="87"/>
+      <c r="C136" s="150"/>
       <c r="D136" s="88"/>
       <c r="E136" s="88"/>
       <c r="F136" s="88"/>
@@ -4741,12 +4801,12 @@
       <c r="J136" s="23"/>
       <c r="K136" s="10"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B137" s="24"/>
-      <c r="C137" s="47">
+      <c r="C137" s="146">
         <v>0</v>
       </c>
       <c r="D137" s="48">
@@ -4770,12 +4830,12 @@
       <c r="J137" s="25"/>
       <c r="K137" s="10"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="24"/>
-      <c r="C138" s="47">
+      <c r="C138" s="146">
         <v>0</v>
       </c>
       <c r="D138" s="48">
@@ -4799,12 +4859,12 @@
       <c r="J138" s="25"/>
       <c r="K138" s="10"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B139" s="24"/>
-      <c r="C139" s="47">
+      <c r="C139" s="146">
         <v>0</v>
       </c>
       <c r="D139" s="48">
@@ -4828,12 +4888,12 @@
       <c r="J139" s="25"/>
       <c r="K139" s="10"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B140" s="24"/>
-      <c r="C140" s="47">
+      <c r="C140" s="146">
         <v>0</v>
       </c>
       <c r="D140" s="48">
@@ -4857,12 +4917,12 @@
       <c r="J140" s="25"/>
       <c r="K140" s="10"/>
     </row>
-    <row r="141" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B141" s="26"/>
-      <c r="C141" s="108">
+      <c r="C141" s="147">
         <v>0</v>
       </c>
       <c r="D141" s="106">
@@ -4886,14 +4946,14 @@
       <c r="J141" s="27"/>
       <c r="K141" s="10"/>
     </row>
-    <row r="142" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B142" s="45">
         <v>0</v>
       </c>
-      <c r="C142" s="90">
+      <c r="C142" s="148">
         <f t="shared" ref="C142:I142" si="15">SUM(C137:C141)</f>
         <v>0</v>
       </c>
@@ -4924,9 +4984,9 @@
       <c r="J142" s="115"/>
       <c r="K142" s="10"/>
     </row>
-    <row r="143" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="28"/>
-      <c r="C143" s="93"/>
+      <c r="C143" s="149"/>
       <c r="D143" s="93"/>
       <c r="E143" s="93"/>
       <c r="F143" s="93"/>
@@ -4935,12 +4995,12 @@
       <c r="I143" s="93"/>
       <c r="J143" s="29"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B144" s="22"/>
-      <c r="C144" s="87"/>
+      <c r="C144" s="150"/>
       <c r="D144" s="88"/>
       <c r="E144" s="88"/>
       <c r="F144" s="88"/>
@@ -4950,12 +5010,12 @@
       <c r="J144" s="23"/>
       <c r="K144" s="10"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B145" s="24"/>
-      <c r="C145" s="47">
+      <c r="C145" s="146">
         <v>0</v>
       </c>
       <c r="D145" s="48">
@@ -4979,12 +5039,12 @@
       <c r="J145" s="25"/>
       <c r="K145" s="10"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B146" s="24"/>
-      <c r="C146" s="47">
+      <c r="C146" s="146">
         <v>0</v>
       </c>
       <c r="D146" s="48">
@@ -5008,12 +5068,12 @@
       <c r="J146" s="25"/>
       <c r="K146" s="10"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B147" s="24"/>
-      <c r="C147" s="47">
+      <c r="C147" s="146">
         <v>0</v>
       </c>
       <c r="D147" s="48">
@@ -5037,12 +5097,12 @@
       <c r="J147" s="25"/>
       <c r="K147" s="10"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B148" s="24"/>
-      <c r="C148" s="47">
+      <c r="C148" s="146">
         <v>0</v>
       </c>
       <c r="D148" s="48">
@@ -5066,12 +5126,12 @@
       <c r="J148" s="25"/>
       <c r="K148" s="10"/>
     </row>
-    <row r="149" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B149" s="26"/>
-      <c r="C149" s="108">
+      <c r="C149" s="147">
         <v>0</v>
       </c>
       <c r="D149" s="106">
@@ -5095,14 +5155,14 @@
       <c r="J149" s="27"/>
       <c r="K149" s="10"/>
     </row>
-    <row r="150" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B150" s="45">
         <v>0</v>
       </c>
-      <c r="C150" s="90">
+      <c r="C150" s="148">
         <f t="shared" ref="C150:I150" si="16">SUM(C145:C149)</f>
         <v>0</v>
       </c>
@@ -5133,8 +5193,8 @@
       <c r="J150" s="38"/>
       <c r="K150" s="10"/>
     </row>
-    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C151" s="93"/>
+    <row r="151" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C151" s="149"/>
       <c r="D151" s="93"/>
       <c r="E151" s="93"/>
       <c r="F151" s="93"/>
@@ -5142,12 +5202,12 @@
       <c r="H151" s="93"/>
       <c r="I151" s="93"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B152" s="8"/>
-      <c r="C152" s="87"/>
+      <c r="C152" s="150"/>
       <c r="D152" s="88"/>
       <c r="E152" s="88"/>
       <c r="F152" s="88"/>
@@ -5157,12 +5217,12 @@
       <c r="J152" s="1"/>
       <c r="K152" s="10"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B153" s="10"/>
-      <c r="C153" s="47">
+      <c r="C153" s="146">
         <v>0</v>
       </c>
       <c r="D153" s="48">
@@ -5186,12 +5246,12 @@
       <c r="J153" s="2"/>
       <c r="K153" s="10"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B154" s="10"/>
-      <c r="C154" s="47">
+      <c r="C154" s="146">
         <v>0</v>
       </c>
       <c r="D154" s="48">
@@ -5215,12 +5275,12 @@
       <c r="J154" s="2"/>
       <c r="K154" s="10"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B155" s="10"/>
-      <c r="C155" s="47">
+      <c r="C155" s="146">
         <v>0</v>
       </c>
       <c r="D155" s="48">
@@ -5244,12 +5304,12 @@
       <c r="J155" s="2"/>
       <c r="K155" s="10"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B156" s="10"/>
-      <c r="C156" s="47">
+      <c r="C156" s="146">
         <v>0</v>
       </c>
       <c r="D156" s="48">
@@ -5273,12 +5333,12 @@
       <c r="J156" s="2"/>
       <c r="K156" s="10"/>
     </row>
-    <row r="157" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B157" s="9"/>
-      <c r="C157" s="108">
+      <c r="C157" s="147">
         <v>0</v>
       </c>
       <c r="D157" s="106">
@@ -5302,14 +5362,14 @@
       <c r="J157" s="3"/>
       <c r="K157" s="10"/>
     </row>
-    <row r="158" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B158" s="45">
         <v>0</v>
       </c>
-      <c r="C158" s="90">
+      <c r="C158" s="148">
         <f t="shared" ref="C158:I158" si="17">SUM(C153:C157)</f>
         <v>0</v>
       </c>
@@ -5340,8 +5400,8 @@
       <c r="J158" s="38"/>
       <c r="K158" s="10"/>
     </row>
-    <row r="159" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C159" s="93"/>
+    <row r="159" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C159" s="149"/>
       <c r="D159" s="93"/>
       <c r="E159" s="93"/>
       <c r="F159" s="93"/>
@@ -5349,12 +5409,12 @@
       <c r="H159" s="93"/>
       <c r="I159" s="93"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B160" s="8"/>
-      <c r="C160" s="87"/>
+      <c r="C160" s="150"/>
       <c r="D160" s="88"/>
       <c r="E160" s="88"/>
       <c r="F160" s="88"/>
@@ -5364,12 +5424,12 @@
       <c r="J160" s="1"/>
       <c r="K160" s="10"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B161" s="10"/>
-      <c r="C161" s="47">
+      <c r="C161" s="146">
         <v>0</v>
       </c>
       <c r="D161" s="48">
@@ -5393,12 +5453,12 @@
       <c r="J161" s="2"/>
       <c r="K161" s="10"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B162" s="10"/>
-      <c r="C162" s="47">
+      <c r="C162" s="146">
         <v>0</v>
       </c>
       <c r="D162" s="48">
@@ -5422,12 +5482,12 @@
       <c r="J162" s="2"/>
       <c r="K162" s="10"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B163" s="10"/>
-      <c r="C163" s="47">
+      <c r="C163" s="146">
         <v>0</v>
       </c>
       <c r="D163" s="48">
@@ -5451,12 +5511,12 @@
       <c r="J163" s="2"/>
       <c r="K163" s="10"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B164" s="10"/>
-      <c r="C164" s="47">
+      <c r="C164" s="146">
         <v>0</v>
       </c>
       <c r="D164" s="48">
@@ -5480,12 +5540,12 @@
       <c r="J164" s="2"/>
       <c r="K164" s="10"/>
     </row>
-    <row r="165" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B165" s="9"/>
-      <c r="C165" s="108">
+      <c r="C165" s="147">
         <v>0</v>
       </c>
       <c r="D165" s="106">
@@ -5509,14 +5569,14 @@
       <c r="J165" s="3"/>
       <c r="K165" s="10"/>
     </row>
-    <row r="166" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B166" s="45">
         <v>0</v>
       </c>
-      <c r="C166" s="90">
+      <c r="C166" s="148">
         <f t="shared" ref="C166:I166" si="18">SUM(C161:C165)</f>
         <v>0</v>
       </c>
@@ -5547,8 +5607,8 @@
       <c r="J166" s="38"/>
       <c r="K166" s="10"/>
     </row>
-    <row r="167" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C167" s="93"/>
+    <row r="167" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C167" s="149"/>
       <c r="D167" s="93"/>
       <c r="E167" s="93"/>
       <c r="F167" s="93"/>
@@ -5556,12 +5616,12 @@
       <c r="H167" s="93"/>
       <c r="I167" s="93"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B168" s="8"/>
-      <c r="C168" s="87"/>
+      <c r="C168" s="150"/>
       <c r="D168" s="88"/>
       <c r="E168" s="88"/>
       <c r="F168" s="88"/>
@@ -5571,12 +5631,12 @@
       <c r="J168" s="1"/>
       <c r="K168" s="10"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B169" s="10"/>
-      <c r="C169" s="47">
+      <c r="C169" s="146">
         <v>0</v>
       </c>
       <c r="D169" s="48">
@@ -5600,12 +5660,12 @@
       <c r="J169" s="2"/>
       <c r="K169" s="10"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B170" s="10"/>
-      <c r="C170" s="47">
+      <c r="C170" s="146">
         <v>0</v>
       </c>
       <c r="D170" s="48">
@@ -5629,12 +5689,12 @@
       <c r="J170" s="2"/>
       <c r="K170" s="10"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B171" s="10"/>
-      <c r="C171" s="47">
+      <c r="C171" s="146">
         <v>0</v>
       </c>
       <c r="D171" s="48">
@@ -5658,12 +5718,12 @@
       <c r="J171" s="2"/>
       <c r="K171" s="10"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B172" s="10"/>
-      <c r="C172" s="47">
+      <c r="C172" s="146">
         <v>0</v>
       </c>
       <c r="D172" s="48">
@@ -5687,12 +5747,12 @@
       <c r="J172" s="2"/>
       <c r="K172" s="10"/>
     </row>
-    <row r="173" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B173" s="9"/>
-      <c r="C173" s="108">
+      <c r="C173" s="147">
         <v>0</v>
       </c>
       <c r="D173" s="106">
@@ -5716,14 +5776,14 @@
       <c r="J173" s="3"/>
       <c r="K173" s="10"/>
     </row>
-    <row r="174" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B174" s="45">
         <v>0</v>
       </c>
-      <c r="C174" s="90">
+      <c r="C174" s="148">
         <f t="shared" ref="C174:I174" si="19">SUM(C169:C173)</f>
         <v>0</v>
       </c>
@@ -5754,7 +5814,7 @@
       <c r="J174" s="38"/>
       <c r="K174" s="10"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C175" s="93"/>
       <c r="D175" s="93"/>
       <c r="E175" s="93"/>

</xml_diff>